<commit_message>
adding a temp password
</commit_message>
<xml_diff>
--- a/students_sample2.xlsx
+++ b/students_sample2.xlsx
@@ -61,10 +61,10 @@
     <t>achala.14@cse.mrt.ac.lk</t>
   </si>
   <si>
-    <t>aijdissanayake@gmail.com</t>
-  </si>
-  <si>
     <t>Achala</t>
+  </si>
+  <si>
+    <t>achalazone@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -412,7 +412,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:I6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -491,10 +491,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="D3">
         <v>7777777778</v>

</xml_diff>